<commit_message>
Established: Main script init
</commit_message>
<xml_diff>
--- a/BTC_data.xlsx
+++ b/BTC_data.xlsx
@@ -474,20 +474,20 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>23.03.2023</t>
+          <t>26.03.2023</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>28310.7</v>
+        <v>27973.5</v>
       </c>
       <c r="F4" t="n">
-        <v>27262.8</v>
+        <v>27474.9</v>
       </c>
       <c r="G4" t="n">
-        <v>28734.1</v>
+        <v>28153.7</v>
       </c>
       <c r="H4" t="n">
-        <v>27144.6</v>
+        <v>27429.1</v>
       </c>
     </row>
     <row r="5">
@@ -499,20 +499,20 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>24.03.2023</t>
+          <t>27.03.2023</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>27462.2</v>
+        <v>27129.8</v>
       </c>
       <c r="F5" t="n">
-        <v>28306.9</v>
+        <v>27974.8</v>
       </c>
       <c r="G5" t="n">
-        <v>28374.5</v>
+        <v>28023.3</v>
       </c>
       <c r="H5" t="n">
-        <v>27026.5</v>
+        <v>26611.5</v>
       </c>
     </row>
     <row r="6">
@@ -524,20 +524,20 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>25.03.2023</t>
+          <t>28.03.2023</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>27475.6</v>
+        <v>27262.2</v>
       </c>
       <c r="F6" t="n">
-        <v>27462.2</v>
+        <v>27127.8</v>
       </c>
       <c r="G6" t="n">
-        <v>27761.9</v>
+        <v>27465</v>
       </c>
       <c r="H6" t="n">
-        <v>27176.7</v>
+        <v>26665.6</v>
       </c>
     </row>
     <row r="7">
@@ -549,20 +549,20 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>26.03.2023</t>
+          <t>29.03.2023</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>27973.5</v>
+        <v>28350.4</v>
       </c>
       <c r="F7" t="n">
-        <v>27474.9</v>
+        <v>27262.9</v>
       </c>
       <c r="G7" t="n">
-        <v>28153.7</v>
+        <v>28627.4</v>
       </c>
       <c r="H7" t="n">
-        <v>27429.1</v>
+        <v>27249.8</v>
       </c>
     </row>
     <row r="8">
@@ -574,20 +574,20 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>27.03.2023</t>
+          <t>30.03.2023</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>27129.8</v>
+        <v>28029.5</v>
       </c>
       <c r="F8" t="n">
-        <v>27974.8</v>
+        <v>28350.3</v>
       </c>
       <c r="G8" t="n">
-        <v>28023.3</v>
+        <v>29160.4</v>
       </c>
       <c r="H8" t="n">
-        <v>26611.5</v>
+        <v>27716.7</v>
       </c>
     </row>
     <row r="9">
@@ -599,20 +599,20 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>28.03.2023</t>
+          <t>31.03.2023</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>27262.2</v>
+        <v>28473.7</v>
       </c>
       <c r="F9" t="n">
-        <v>27127.8</v>
+        <v>28029.3</v>
       </c>
       <c r="G9" t="n">
-        <v>27465</v>
+        <v>28646.3</v>
       </c>
       <c r="H9" t="n">
-        <v>26665.6</v>
+        <v>27587.5</v>
       </c>
     </row>
     <row r="10">
@@ -624,20 +624,20 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>29.03.2023</t>
+          <t>01.04.2023</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>28350.4</v>
+        <v>28456.1</v>
       </c>
       <c r="F10" t="n">
-        <v>27262.9</v>
+        <v>28473.7</v>
       </c>
       <c r="G10" t="n">
-        <v>28627.4</v>
+        <v>28795.1</v>
       </c>
       <c r="H10" t="n">
-        <v>27249.8</v>
+        <v>28285.6</v>
       </c>
     </row>
     <row r="11">
@@ -649,20 +649,20 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>30.03.2023</t>
+          <t>02.04.2023</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>28029.5</v>
+        <v>28198.3</v>
       </c>
       <c r="F11" t="n">
-        <v>28350.3</v>
+        <v>28456.1</v>
       </c>
       <c r="G11" t="n">
-        <v>29160.4</v>
+        <v>28522.8</v>
       </c>
       <c r="H11" t="n">
-        <v>27716.7</v>
+        <v>27871.7</v>
       </c>
     </row>
     <row r="12">
@@ -674,20 +674,20 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>31.03.2023</t>
+          <t>03.04.2023</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>28473.7</v>
+        <v>27802.1</v>
       </c>
       <c r="F12" t="n">
-        <v>28029.3</v>
+        <v>28194.7</v>
       </c>
       <c r="G12" t="n">
-        <v>28646.3</v>
+        <v>28458.4</v>
       </c>
       <c r="H12" t="n">
-        <v>27587.5</v>
+        <v>27256.9</v>
       </c>
     </row>
     <row r="13">
@@ -699,20 +699,20 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>01.04.2023</t>
+          <t>04.04.2023</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>28456.1</v>
+        <v>28164.4</v>
       </c>
       <c r="F13" t="n">
-        <v>28473.7</v>
+        <v>27802.2</v>
       </c>
       <c r="G13" t="n">
-        <v>28795.1</v>
+        <v>28429.1</v>
       </c>
       <c r="H13" t="n">
-        <v>28285.6</v>
+        <v>27668.9</v>
       </c>
     </row>
     <row r="14">
@@ -724,20 +724,20 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>02.04.2023</t>
+          <t>05.04.2023</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>28198.3</v>
+        <v>28173.5</v>
       </c>
       <c r="F14" t="n">
-        <v>28456.1</v>
+        <v>28164.4</v>
       </c>
       <c r="G14" t="n">
-        <v>28522.8</v>
+        <v>28744.4</v>
       </c>
       <c r="H14" t="n">
-        <v>27871.7</v>
+        <v>27823.5</v>
       </c>
     </row>
     <row r="15">
@@ -749,20 +749,20 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>03.04.2023</t>
+          <t>06.04.2023</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>27802.1</v>
+        <v>28036.7</v>
       </c>
       <c r="F15" t="n">
-        <v>28194.7</v>
+        <v>28173.5</v>
       </c>
       <c r="G15" t="n">
-        <v>28458.4</v>
+        <v>28173.5</v>
       </c>
       <c r="H15" t="n">
-        <v>27256.9</v>
+        <v>27734.5</v>
       </c>
     </row>
     <row r="16">
@@ -774,20 +774,20 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>04.04.2023</t>
+          <t>07.04.2023</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>28164.4</v>
+        <v>27910.4</v>
       </c>
       <c r="F16" t="n">
-        <v>27802.2</v>
+        <v>28037.6</v>
       </c>
       <c r="G16" t="n">
-        <v>28429.1</v>
+        <v>28102.5</v>
       </c>
       <c r="H16" t="n">
-        <v>27668.9</v>
+        <v>27779.4</v>
       </c>
     </row>
     <row r="17">
@@ -799,20 +799,20 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>05.04.2023</t>
+          <t>08.04.2023</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>28173.5</v>
+        <v>27941.2</v>
       </c>
       <c r="F17" t="n">
-        <v>28164.4</v>
+        <v>27910.4</v>
       </c>
       <c r="G17" t="n">
-        <v>28744.4</v>
+        <v>28153.1</v>
       </c>
       <c r="H17" t="n">
-        <v>27823.5</v>
+        <v>27863.8</v>
       </c>
     </row>
     <row r="18">
@@ -824,20 +824,20 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>06.04.2023</t>
+          <t>09.04.2023</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>28036.7</v>
+        <v>28326.6</v>
       </c>
       <c r="F18" t="n">
-        <v>28173.5</v>
+        <v>27941.2</v>
       </c>
       <c r="G18" t="n">
-        <v>28173.5</v>
+        <v>28522.7</v>
       </c>
       <c r="H18" t="n">
-        <v>27734.5</v>
+        <v>27809.2</v>
       </c>
     </row>
     <row r="19">
@@ -849,20 +849,20 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>07.04.2023</t>
+          <t>10.04.2023</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>27910.4</v>
+        <v>29641</v>
       </c>
       <c r="F19" t="n">
-        <v>28037.6</v>
+        <v>28326.5</v>
       </c>
       <c r="G19" t="n">
-        <v>28102.5</v>
+        <v>29755.4</v>
       </c>
       <c r="H19" t="n">
-        <v>27779.4</v>
+        <v>28182.9</v>
       </c>
     </row>
     <row r="20">
@@ -874,20 +874,20 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>08.04.2023</t>
+          <t>11.04.2023</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>27941.2</v>
+        <v>30209.6</v>
       </c>
       <c r="F20" t="n">
-        <v>27910.4</v>
+        <v>29641</v>
       </c>
       <c r="G20" t="n">
-        <v>28153.1</v>
+        <v>30484.6</v>
       </c>
       <c r="H20" t="n">
-        <v>27863.8</v>
+        <v>29597.8</v>
       </c>
     </row>
     <row r="21">
@@ -899,20 +899,20 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>09.04.2023</t>
+          <t>12.04.2023</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>28326.6</v>
+        <v>29886.4</v>
       </c>
       <c r="F21" t="n">
-        <v>27941.2</v>
+        <v>30209.8</v>
       </c>
       <c r="G21" t="n">
-        <v>28522.7</v>
+        <v>30473</v>
       </c>
       <c r="H21" t="n">
-        <v>27809.2</v>
+        <v>29679.5</v>
       </c>
     </row>
     <row r="22">
@@ -924,20 +924,20 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>10.04.2023</t>
+          <t>13.04.2023</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>29641</v>
+        <v>30387.4</v>
       </c>
       <c r="F22" t="n">
-        <v>28326.5</v>
+        <v>29892.4</v>
       </c>
       <c r="G22" t="n">
-        <v>29755.4</v>
+        <v>30524.1</v>
       </c>
       <c r="H22" t="n">
-        <v>28182.9</v>
+        <v>29864.5</v>
       </c>
     </row>
     <row r="23">
@@ -949,20 +949,20 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>11.04.2023</t>
+          <t>14.04.2023</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>30209.6</v>
+        <v>30472.5</v>
       </c>
       <c r="F23" t="n">
-        <v>29641</v>
+        <v>30387.4</v>
       </c>
       <c r="G23" t="n">
-        <v>30484.6</v>
+        <v>30964.9</v>
       </c>
       <c r="H23" t="n">
-        <v>29597.8</v>
+        <v>30026</v>
       </c>
     </row>
     <row r="24">
@@ -974,20 +974,20 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12.04.2023</t>
+          <t>15.04.2023</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>29886.4</v>
+        <v>30299.6</v>
       </c>
       <c r="F24" t="n">
-        <v>30209.8</v>
+        <v>30472.6</v>
       </c>
       <c r="G24" t="n">
-        <v>30473</v>
+        <v>30586.5</v>
       </c>
       <c r="H24" t="n">
-        <v>29679.5</v>
+        <v>30208.8</v>
       </c>
     </row>
     <row r="25">
@@ -999,20 +999,20 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13.04.2023</t>
+          <t>16.04.2023</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>30387.4</v>
+        <v>30310.3</v>
       </c>
       <c r="F25" t="n">
-        <v>29892.4</v>
+        <v>30299.2</v>
       </c>
       <c r="G25" t="n">
-        <v>30524.1</v>
+        <v>30545.3</v>
       </c>
       <c r="H25" t="n">
-        <v>29864.5</v>
+        <v>30134.6</v>
       </c>
     </row>
     <row r="26">
@@ -1024,20 +1024,20 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14.04.2023</t>
+          <t>17.04.2023</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>30472.5</v>
+        <v>29434.9</v>
       </c>
       <c r="F26" t="n">
-        <v>30387.4</v>
+        <v>30310.8</v>
       </c>
       <c r="G26" t="n">
-        <v>30964.9</v>
+        <v>30312.2</v>
       </c>
       <c r="H26" t="n">
-        <v>30026</v>
+        <v>29274</v>
       </c>
     </row>
     <row r="27">
@@ -1049,20 +1049,20 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>15.04.2023</t>
+          <t>18.04.2023</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>30299.6</v>
+        <v>30382.2</v>
       </c>
       <c r="F27" t="n">
-        <v>30472.6</v>
+        <v>29434.1</v>
       </c>
       <c r="G27" t="n">
-        <v>30586.5</v>
+        <v>30470.1</v>
       </c>
       <c r="H27" t="n">
-        <v>30208.8</v>
+        <v>29149.2</v>
       </c>
     </row>
     <row r="28">
@@ -1074,20 +1074,20 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>16.04.2023</t>
+          <t>19.04.2023</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>30310.3</v>
+        <v>28813.7</v>
       </c>
       <c r="F28" t="n">
-        <v>30299.2</v>
+        <v>30382.2</v>
       </c>
       <c r="G28" t="n">
-        <v>30545.3</v>
+        <v>30408.4</v>
       </c>
       <c r="H28" t="n">
-        <v>30134.6</v>
+        <v>28641.1</v>
       </c>
     </row>
     <row r="29">
@@ -1099,20 +1099,20 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>17.04.2023</t>
+          <t>20.04.2023</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>29434.9</v>
+        <v>28240.5</v>
       </c>
       <c r="F29" t="n">
-        <v>30310.8</v>
+        <v>28813.7</v>
       </c>
       <c r="G29" t="n">
-        <v>30312.2</v>
+        <v>29082.1</v>
       </c>
       <c r="H29" t="n">
-        <v>29274</v>
+        <v>28032.4</v>
       </c>
     </row>
     <row r="30">
@@ -1124,20 +1124,20 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>18.04.2023</t>
+          <t>21.04.2023</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>30382.2</v>
+        <v>27264.8</v>
       </c>
       <c r="F30" t="n">
-        <v>29434.1</v>
+        <v>28240.5</v>
       </c>
       <c r="G30" t="n">
-        <v>30470.1</v>
+        <v>28353.4</v>
       </c>
       <c r="H30" t="n">
-        <v>29149.2</v>
+        <v>27171.1</v>
       </c>
     </row>
     <row r="31">
@@ -1149,20 +1149,20 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>19.04.2023</t>
+          <t>22.04.2023</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>28813.7</v>
+        <v>27813.9</v>
       </c>
       <c r="F31" t="n">
-        <v>30382.2</v>
+        <v>27264.8</v>
       </c>
       <c r="G31" t="n">
-        <v>30408.4</v>
+        <v>27872</v>
       </c>
       <c r="H31" t="n">
-        <v>28641.1</v>
+        <v>27165.7</v>
       </c>
     </row>
     <row r="32">
@@ -1174,20 +1174,20 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>20.04.2023</t>
+          <t>23.04.2023</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>28240.5</v>
+        <v>27591.4</v>
       </c>
       <c r="F32" t="n">
-        <v>28813.7</v>
+        <v>27813.8</v>
       </c>
       <c r="G32" t="n">
-        <v>29082.1</v>
+        <v>27815</v>
       </c>
       <c r="H32" t="n">
-        <v>28032.4</v>
+        <v>27388.5</v>
       </c>
     </row>
     <row r="33">
@@ -1199,20 +1199,20 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>21.04.2023</t>
+          <t>24.04.2023</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>27264.8</v>
+        <v>27509.3</v>
       </c>
       <c r="F33" t="n">
-        <v>28240.5</v>
+        <v>27591.4</v>
       </c>
       <c r="G33" t="n">
-        <v>28353.4</v>
+        <v>27978.8</v>
       </c>
       <c r="H33" t="n">
-        <v>27171.1</v>
+        <v>27054.3</v>
       </c>
     </row>
     <row r="34">
@@ -1224,20 +1224,20 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>22.04.2023</t>
+          <t>25.04.2023</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>27813.9</v>
+        <v>28298.8</v>
       </c>
       <c r="F34" t="n">
-        <v>27264.8</v>
+        <v>27510.1</v>
       </c>
       <c r="G34" t="n">
-        <v>27872</v>
+        <v>28375.6</v>
       </c>
       <c r="H34" t="n">
-        <v>27165.7</v>
+        <v>27201.1</v>
       </c>
     </row>
     <row r="35">
@@ -1249,20 +1249,20 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>23.04.2023</t>
+          <t>26.04.2023</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>27431.7</v>
+        <v>28341.2</v>
       </c>
       <c r="F35" t="n">
-        <v>27813.8</v>
+        <v>28298.8</v>
       </c>
       <c r="G35" t="n">
-        <v>27815</v>
+        <v>29995.7</v>
       </c>
       <c r="H35" t="n">
-        <v>27393.1</v>
+        <v>27307.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>